<commit_message>
Etude des livres de recherche opérationnelle - management science
</commit_message>
<xml_diff>
--- a/01. Recherche opérationnelle (Operations research - Management science)/Etude des livres.xlsx
+++ b/01. Recherche opérationnelle (Operations research - Management science)/Etude des livres.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="32">
   <si>
     <t>Optimization Modeling with Spreadsheets</t>
   </si>
@@ -75,42 +75,51 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">COURSERA
+    <t>Introduction au modeling</t>
+  </si>
+  <si>
+    <t>Déterminer le meilleur prix break even( relation entre prix et volume de vente) non linéaire avec le fichier excel +   explication de l'analyse de sensitivité + méthode du solveur excel</t>
+  </si>
+  <si>
+    <t>non</t>
+  </si>
+  <si>
+    <t>tradeoff</t>
+  </si>
+  <si>
+    <t>compromis</t>
+  </si>
+  <si>
+    <t>Programmation non linéaire</t>
+  </si>
+  <si>
+    <t>Fonction convexe</t>
+  </si>
+  <si>
+    <t>fonction en forme de U</t>
+  </si>
+  <si>
+    <t>Foncion concave</t>
+  </si>
+  <si>
+    <t>Fonction en forme de montagne</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 minimise le coût annuel de commande et d'inventaire
+2 Un exemple de remise sur quantité                                                                                                                                3 Facility location en 2 dimensions                                                                                                                                      4 Pricing non linéaire                                                                                                                                                                5 sensitivité des programmes non linéaires                                                                                                                      6 Le portfolio                                                                                                                                                                                7 Comment linéariser
 </t>
   </si>
   <si>
-    <t>Introduction au modeling</t>
-  </si>
-  <si>
-    <t>Déterminer le meilleur prix break even( relation entre prix et volume de vente) non linéaire avec le fichier excel +   explication de l'analyse de sensitivité + méthode du solveur excel</t>
-  </si>
-  <si>
-    <t>non</t>
-  </si>
-  <si>
-    <t>tradeoff</t>
-  </si>
-  <si>
-    <t>compromis</t>
-  </si>
-  <si>
-    <t>Programmation non linéaire</t>
-  </si>
-  <si>
-    <t>Fonction convexe</t>
-  </si>
-  <si>
-    <t>fonction en forme de U</t>
-  </si>
-  <si>
-    <t>Foncion concave</t>
-  </si>
-  <si>
-    <t>Fonction en forme de montagne</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 minimise le coût annuel de commande et d'inventaire
-2 Un exemple de remise sur quantité                                                                                                                                3 Facility location en 2 dimensions                                                                                                                                      4 Pricing non linéaire                                                                                                                                                                5 sensitivité des programmes non linéaires                                                                                                                      6 Le portfolio
+    <t>Introduction to Linear Programming</t>
+  </si>
+  <si>
+    <t>Bernard_W_._Taylor_Introduction_to_Management_Science_11th_2013</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [Roberta_S._Russell,_Bernard_W._Taylor]_Operations(Bookos.org)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COURSERA Taiwan university - Operations research
 </t>
   </si>
 </sst>
@@ -188,7 +197,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -200,6 +209,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -480,10 +495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:E46"/>
+  <dimension ref="A3:E79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -503,7 +518,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
+      <c r="D3" s="7"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
@@ -513,7 +528,7 @@
       <c r="C4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="5" t="s">
         <v>2</v>
       </c>
       <c r="E4" s="3" t="s">
@@ -525,14 +540,14 @@
         <v>1</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -589,18 +604,26 @@
       <c r="D11" s="5"/>
       <c r="E11" s="3"/>
     </row>
-    <row r="12" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E12" s="3"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D13" s="8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D14" s="8"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
@@ -610,7 +633,7 @@
         <v>13</v>
       </c>
       <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
+      <c r="D15" s="7"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
@@ -620,7 +643,7 @@
       <c r="C16" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="5" t="s">
         <v>2</v>
       </c>
       <c r="E16" s="3" t="s">
@@ -633,7 +656,7 @@
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
+      <c r="D17" s="5"/>
       <c r="E17" s="3"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -642,7 +665,7 @@
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
+      <c r="D18" s="5"/>
       <c r="E18" s="3"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -651,7 +674,7 @@
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
+      <c r="D19" s="5"/>
       <c r="E19" s="3"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -660,7 +683,7 @@
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
+      <c r="D20" s="5"/>
       <c r="E20" s="3"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -669,7 +692,7 @@
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
+      <c r="D21" s="5"/>
       <c r="E21" s="3"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -678,7 +701,7 @@
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
+      <c r="D22" s="5"/>
       <c r="E22" s="3"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -687,7 +710,7 @@
       </c>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
+      <c r="D23" s="5"/>
       <c r="E23" s="3"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -696,8 +719,11 @@
       </c>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
+      <c r="D24" s="5"/>
       <c r="E24" s="3"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D25" s="8"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
@@ -707,7 +733,7 @@
         <v>14</v>
       </c>
       <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
+      <c r="D26" s="7"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
@@ -717,7 +743,7 @@
       <c r="C27" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="D27" s="5" t="s">
         <v>2</v>
       </c>
       <c r="E27" s="3" t="s">
@@ -730,7 +756,7 @@
       </c>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
+      <c r="D28" s="5"/>
       <c r="E28" s="3"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -739,7 +765,7 @@
       </c>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
+      <c r="D29" s="5"/>
       <c r="E29" s="3"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -748,7 +774,7 @@
       </c>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
+      <c r="D30" s="5"/>
       <c r="E30" s="3"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -757,7 +783,7 @@
       </c>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
+      <c r="D31" s="5"/>
       <c r="E31" s="3"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -766,7 +792,7 @@
       </c>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
+      <c r="D32" s="5"/>
       <c r="E32" s="3"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -775,7 +801,7 @@
       </c>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
+      <c r="D33" s="5"/>
       <c r="E33" s="3"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -784,7 +810,7 @@
       </c>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
+      <c r="D34" s="5"/>
       <c r="E34" s="3"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -793,8 +819,11 @@
       </c>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
+      <c r="D35" s="5"/>
       <c r="E35" s="3"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D36" s="8"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
@@ -804,7 +833,7 @@
         <v>15</v>
       </c>
       <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
+      <c r="D37" s="7"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
@@ -814,7 +843,7 @@
       <c r="C38" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D38" s="3" t="s">
+      <c r="D38" s="5" t="s">
         <v>2</v>
       </c>
       <c r="E38" s="3" t="s">
@@ -827,7 +856,7 @@
       </c>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
+      <c r="D39" s="5"/>
       <c r="E39" s="3"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -836,7 +865,7 @@
       </c>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
+      <c r="D40" s="5"/>
       <c r="E40" s="3"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -845,7 +874,7 @@
       </c>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
+      <c r="D41" s="5"/>
       <c r="E41" s="3"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -854,7 +883,7 @@
       </c>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
-      <c r="D42" s="3"/>
+      <c r="D42" s="5"/>
       <c r="E42" s="3"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -863,7 +892,7 @@
       </c>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
-      <c r="D43" s="3"/>
+      <c r="D43" s="5"/>
       <c r="E43" s="3"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -872,7 +901,7 @@
       </c>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
+      <c r="D44" s="5"/>
       <c r="E44" s="3"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -881,7 +910,7 @@
       </c>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
-      <c r="D45" s="3"/>
+      <c r="D45" s="5"/>
       <c r="E45" s="3"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -890,8 +919,275 @@
       </c>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
-      <c r="D46" s="3"/>
+      <c r="D46" s="5"/>
       <c r="E46" s="3"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D47" s="8"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>5</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C48" s="1"/>
+      <c r="D48" s="7"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="3"/>
+      <c r="B49" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B50" s="3"/>
+      <c r="C50" s="3"/>
+      <c r="D50" s="5"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B51" s="3"/>
+      <c r="C51" s="3"/>
+      <c r="D51" s="5"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B52" s="3"/>
+      <c r="C52" s="3"/>
+      <c r="D52" s="5"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B53" s="3"/>
+      <c r="C53" s="3"/>
+      <c r="D53" s="5"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B54" s="3"/>
+      <c r="C54" s="3"/>
+      <c r="D54" s="5"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B55" s="3"/>
+      <c r="C55" s="3"/>
+      <c r="D55" s="5"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B56" s="3"/>
+      <c r="C56" s="3"/>
+      <c r="D56" s="5"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B57" s="3"/>
+      <c r="C57" s="3"/>
+      <c r="D57" s="5"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D58" s="8"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="1">
+        <v>6</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C59" s="1"/>
+      <c r="D59" s="7"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="3"/>
+      <c r="B60" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B61" s="3"/>
+      <c r="C61" s="3"/>
+      <c r="D61" s="5"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B62" s="3"/>
+      <c r="C62" s="3"/>
+      <c r="D62" s="5"/>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B63" s="3"/>
+      <c r="C63" s="3"/>
+      <c r="D63" s="5"/>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B64" s="3"/>
+      <c r="C64" s="3"/>
+      <c r="D64" s="5"/>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B65" s="3"/>
+      <c r="C65" s="3"/>
+      <c r="D65" s="5"/>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B66" s="3"/>
+      <c r="C66" s="3"/>
+      <c r="D66" s="5"/>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B67" s="3"/>
+      <c r="C67" s="3"/>
+      <c r="D67" s="5"/>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B68" s="3"/>
+      <c r="C68" s="3"/>
+      <c r="D68" s="5"/>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D69" s="8"/>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="1">
+        <v>6</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C70" s="1"/>
+      <c r="D70" s="7"/>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="3"/>
+      <c r="B71" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D71" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B72" s="3"/>
+      <c r="C72" s="3"/>
+      <c r="D72" s="5"/>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B73" s="3"/>
+      <c r="C73" s="3"/>
+      <c r="D73" s="5"/>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B74" s="3"/>
+      <c r="C74" s="3"/>
+      <c r="D74" s="5"/>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B75" s="3"/>
+      <c r="C75" s="3"/>
+      <c r="D75" s="5"/>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B76" s="3"/>
+      <c r="C76" s="3"/>
+      <c r="D76" s="5"/>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B77" s="3"/>
+      <c r="C77" s="3"/>
+      <c r="D77" s="5"/>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B78" s="3"/>
+      <c r="C78" s="3"/>
+      <c r="D78" s="5"/>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B79" s="3"/>
+      <c r="C79" s="3"/>
+      <c r="D79" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -903,7 +1199,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13:C14"/>
+      <selection activeCell="B17" sqref="B16:B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1011,12 +1307,12 @@
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
     </row>
-    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>1</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -1128,26 +1424,26 @@
   <sheetData>
     <row r="1" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
         <v>21</v>
-      </c>
-      <c r="B1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
         <v>24</v>
-      </c>
-      <c r="B2" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s">
         <v>26</v>
-      </c>
-      <c r="B3" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ajout du cours de Columbia Business School university - Decisions models
</commit_message>
<xml_diff>
--- a/01. Recherche opérationnelle (Operations research - Management science)/Etude des livres.xlsx
+++ b/01. Recherche opérationnelle (Operations research - Management science)/Etude des livres.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LIVRES" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="81">
   <si>
     <t>Optimization Modeling with Spreadsheets</t>
   </si>
@@ -323,6 +323,10 @@
   </si>
   <si>
     <t>Exercices</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Colombia Business school University - Operations research -Decisions models
+</t>
   </si>
 </sst>
 </file>
@@ -756,8 +760,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="A68" sqref="A68:XFD68"/>
+    <sheetView topLeftCell="A72" workbookViewId="0">
+      <selection activeCell="A80" sqref="A80:D89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1742,10 +1746,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B16:B17"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1949,6 +1953,103 @@
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
+    </row>
+    <row r="23" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>1</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Ajout du cours de Bernard Fortz
</commit_message>
<xml_diff>
--- a/01. Recherche opérationnelle (Operations research - Management science)/Etude des livres.xlsx
+++ b/01. Recherche opérationnelle (Operations research - Management science)/Etude des livres.xlsx
@@ -10,6 +10,7 @@
     <sheet name="LIVRES" sheetId="1" r:id="rId1"/>
     <sheet name="COURS" sheetId="2" r:id="rId2"/>
     <sheet name="vocabulaire" sheetId="3" r:id="rId3"/>
+    <sheet name="Livres théorie mathématique" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="83">
   <si>
     <t>Optimization Modeling with Spreadsheets</t>
   </si>
@@ -326,6 +327,13 @@
   </si>
   <si>
     <t xml:space="preserve">Colombia Business school University - Operations research -Decisions models
+</t>
+  </si>
+  <si>
+    <t>Livre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recherche opérationnelle et applications - Bernard Fortz
 </t>
   </si>
 </sst>
@@ -1746,10 +1754,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1859,7 +1867,7 @@
     </row>
     <row r="12" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>28</v>
@@ -1956,7 +1964,7 @@
     </row>
     <row r="23" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>80</v>
@@ -2050,6 +2058,103 @@
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
+    </row>
+    <row r="34" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>4</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="3"/>
+      <c r="B35" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B41" s="3"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B43" s="3"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2096,4 +2201,22 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>